<commit_message>
add powerflows with EV
</commit_message>
<xml_diff>
--- a/data/EV Calculation.xlsx
+++ b/data/EV Calculation.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27618"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/emile_marien_student_kuleuven_be/Documents/Emile/Unief/MA 1 - Sem 2/2024_spring_P&amp;O_6/MA1SEM2_EnergyProject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1448" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8A1B3A3-9734-4857-B82D-F05CD165754C}"/>
+  <xr:revisionPtr revIDLastSave="1475" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8904C60A-AE88-9A42-9B2C-FFB28CDBA466}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="No smart charging" sheetId="3" r:id="rId2"/>
     <sheet name="Smart charging" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,7 +31,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
-  <si>
-    <t>Datetime</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>Hour</t>
   </si>
@@ -49,31 +46,7 @@
     <t>Day</t>
   </si>
   <si>
-    <t>Load_EV_kW_no_SC</t>
-  </si>
-  <si>
-    <t>Load_EV_kW_SC</t>
-  </si>
-  <si>
-    <t>Charging_type_EV_B2C</t>
-  </si>
-  <si>
-    <t>Week</t>
-  </si>
-  <si>
-    <t>Correction_factor</t>
-  </si>
-  <si>
     <t>Monday</t>
-  </si>
-  <si>
-    <t>charging</t>
-  </si>
-  <si>
-    <t>uncharging</t>
-  </si>
-  <si>
-    <t>disconnected</t>
   </si>
   <si>
     <t>Tuesday</t>
@@ -142,16 +115,76 @@
     <t>Charging time</t>
   </si>
   <si>
+    <t>Datetime</t>
+  </si>
+  <si>
+    <t>Load_EV_kW_no_SC</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Correction_factor</t>
+  </si>
+  <si>
+    <t>Load_EV_kW_SC</t>
+  </si>
+  <si>
+    <t>charging</t>
+  </si>
+  <si>
+    <t>uncharging</t>
+  </si>
+  <si>
+    <t>disconnected</t>
+  </si>
+  <si>
     <t>Average charging load</t>
+  </si>
+  <si>
+    <t>Ratio to max power</t>
   </si>
   <si>
     <t>Average charge</t>
   </si>
   <si>
-    <t>Ratio to max power</t>
+    <t>Charging_type_EV_B2C</t>
   </si>
   <si>
     <t>Period</t>
+  </si>
+  <si>
+    <t>B2G</t>
+  </si>
+  <si>
+    <t>max battery:</t>
+  </si>
+  <si>
+    <t>max cap</t>
+  </si>
+  <si>
+    <t>kWH</t>
+  </si>
+  <si>
+    <t>driving loss</t>
+  </si>
+  <si>
+    <t>household loss</t>
+  </si>
+  <si>
+    <t>end of day power</t>
+  </si>
+  <si>
+    <t>to be added overnight to bring back to 80%:</t>
+  </si>
+  <si>
+    <t>Max charging power:</t>
+  </si>
+  <si>
+    <t>hours needed:</t>
+  </si>
+  <si>
+    <t>kW</t>
   </si>
 </sst>
 </file>
@@ -162,7 +195,7 @@
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,48 +600,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03086007-FF13-4F03-A8AB-B476DD27065A}">
   <dimension ref="A1:H169"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>43101</v>
       </c>
@@ -616,7 +649,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3">
         <f>0</f>
@@ -627,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G2" s="10">
         <v>1</v>
@@ -636,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>43101.041666666664</v>
       </c>
@@ -652,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G3" s="10">
         <v>2</v>
@@ -661,7 +694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>43101.083333333336</v>
       </c>
@@ -677,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G4" s="10">
         <v>3</v>
@@ -686,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>43101.124999826388</v>
       </c>
@@ -709,7 +742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>43101.166666435187</v>
       </c>
@@ -732,7 +765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>43101.208333043978</v>
       </c>
@@ -755,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>43101.249999652777</v>
       </c>
@@ -778,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>43101.291666261575</v>
       </c>
@@ -801,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>43101.333332870374</v>
       </c>
@@ -824,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>43101.374999479165</v>
       </c>
@@ -847,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>43101.416666087964</v>
       </c>
@@ -870,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>43101.458332696762</v>
       </c>
@@ -893,7 +926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>43101.499999305554</v>
       </c>
@@ -916,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>43101.541665914352</v>
       </c>
@@ -939,7 +972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>43101.583332523151</v>
       </c>
@@ -962,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>43101.624999131942</v>
       </c>
@@ -985,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>43101.66666574074</v>
       </c>
@@ -1008,7 +1041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>43101.708332349539</v>
       </c>
@@ -1031,7 +1064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>43101.74999895833</v>
       </c>
@@ -1054,7 +1087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>43101.791665567129</v>
       </c>
@@ -1077,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>43101.833332175927</v>
       </c>
@@ -1100,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>43101.874998784719</v>
       </c>
@@ -1123,7 +1156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>43101.916665393517</v>
       </c>
@@ -1146,7 +1179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>43101.958332002316</v>
       </c>
@@ -1169,7 +1202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>43101.999998611114</v>
       </c>
@@ -1177,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D26" s="3">
         <f>0</f>
@@ -1195,7 +1228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>43102.041665219906</v>
       </c>
@@ -1218,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>43102.083331828704</v>
       </c>
@@ -1241,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>43102.124998437503</v>
       </c>
@@ -1264,7 +1297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>43102.166665046294</v>
       </c>
@@ -1287,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
         <v>43102.208331655092</v>
       </c>
@@ -1310,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
         <v>43102.249998263891</v>
       </c>
@@ -1333,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>43102.291664872682</v>
       </c>
@@ -1355,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <v>43102.333331481481</v>
       </c>
@@ -1377,7 +1410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
         <v>43102.374998090279</v>
       </c>
@@ -1399,7 +1432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
         <v>43102.416664699071</v>
       </c>
@@ -1421,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <v>43102.458331307869</v>
       </c>
@@ -1443,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>43102.499997916668</v>
       </c>
@@ -1465,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
         <v>43102.541664525466</v>
       </c>
@@ -1487,7 +1520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
         <v>43102.583331134258</v>
       </c>
@@ -1509,7 +1542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
         <v>43102.624997743056</v>
       </c>
@@ -1531,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
         <v>43102.666664351855</v>
       </c>
@@ -1553,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
         <v>43102.708330960646</v>
       </c>
@@ -1575,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
         <v>43102.749997569445</v>
       </c>
@@ -1597,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
         <v>43102.791664178243</v>
       </c>
@@ -1619,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
         <v>43102.833330787034</v>
       </c>
@@ -1641,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
         <v>43102.874997395833</v>
       </c>
@@ -1663,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
         <v>43102.916664004631</v>
       </c>
@@ -1685,7 +1718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="11">
         <v>43102.958330613423</v>
       </c>
@@ -1707,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="11">
         <v>43102.999997222221</v>
       </c>
@@ -1715,7 +1748,7 @@
         <v>1.99999999999998</v>
       </c>
       <c r="C50" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D50" s="3">
         <f>0</f>
@@ -1732,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="11">
         <v>43103.04166383102</v>
       </c>
@@ -1754,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="11">
         <v>43103.083330439818</v>
       </c>
@@ -1776,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="11">
         <v>43103.12499704861</v>
       </c>
@@ -1798,7 +1831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="11">
         <v>43103.166663657408</v>
       </c>
@@ -1817,7 +1850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="11">
         <v>43103.208330266207</v>
       </c>
@@ -1836,7 +1869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="11">
         <v>43103.249996874998</v>
       </c>
@@ -1855,7 +1888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="11">
         <v>43103.291663483797</v>
       </c>
@@ -1874,7 +1907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="11">
         <v>43103.333330092595</v>
       </c>
@@ -1893,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="11">
         <v>43103.374996701386</v>
       </c>
@@ -1912,7 +1945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="11">
         <v>43103.416663310185</v>
       </c>
@@ -1931,7 +1964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="11">
         <v>43103.458329918984</v>
       </c>
@@ -1950,7 +1983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="11">
         <v>43103.499996527775</v>
       </c>
@@ -1969,7 +2002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="11">
         <v>43103.541663136573</v>
       </c>
@@ -1988,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="11">
         <v>43103.583329745372</v>
       </c>
@@ -2007,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="11">
         <v>43103.624996354163</v>
       </c>
@@ -2026,7 +2059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="11">
         <v>43103.666662962962</v>
       </c>
@@ -2045,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="11">
         <v>43103.70832957176</v>
       </c>
@@ -2064,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="11">
         <v>43103.749996180559</v>
       </c>
@@ -2083,7 +2116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="11">
         <v>43103.79166278935</v>
       </c>
@@ -2102,7 +2135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="11">
         <v>43103.833329398149</v>
       </c>
@@ -2121,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="11">
         <v>43103.874996006947</v>
       </c>
@@ -2140,7 +2173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="11">
         <v>43103.916662615738</v>
       </c>
@@ -2159,7 +2192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="11">
         <v>43103.958329224537</v>
       </c>
@@ -2179,7 +2212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="11">
         <v>43103.999995833336</v>
       </c>
@@ -2187,7 +2220,7 @@
         <v>2.99999999999996</v>
       </c>
       <c r="C74" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D74" s="3">
         <f>0</f>
@@ -2202,7 +2235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="11">
         <v>43104.041662442127</v>
       </c>
@@ -2222,7 +2255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="11">
         <v>43104.083329050925</v>
       </c>
@@ -2242,7 +2275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="11">
         <v>43104.124995659724</v>
       </c>
@@ -2262,7 +2295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="11">
         <v>43104.166662268515</v>
       </c>
@@ -2282,7 +2315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="11">
         <v>43104.208328877314</v>
       </c>
@@ -2302,7 +2335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="11">
         <v>43104.249995486112</v>
       </c>
@@ -2322,7 +2355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="11">
         <v>43104.291662094911</v>
       </c>
@@ -2342,7 +2375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="11">
         <v>43104.333328703702</v>
       </c>
@@ -2362,7 +2395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="11">
         <v>43104.374995312501</v>
       </c>
@@ -2382,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="11">
         <v>43104.416661921299</v>
       </c>
@@ -2402,7 +2435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="11">
         <v>43104.458328530091</v>
       </c>
@@ -2422,7 +2455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="11">
         <v>43104.499995138889</v>
       </c>
@@ -2442,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="11">
         <v>43104.541661747688</v>
       </c>
@@ -2462,7 +2495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="11">
         <v>43104.583328356479</v>
       </c>
@@ -2482,7 +2515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="11">
         <v>43104.624994965277</v>
       </c>
@@ -2502,7 +2535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="11">
         <v>43104.666661574076</v>
       </c>
@@ -2522,7 +2555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="11">
         <v>43104.708328182867</v>
       </c>
@@ -2542,7 +2575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="11">
         <v>43104.749994791666</v>
       </c>
@@ -2562,7 +2595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="11">
         <v>43104.791661400464</v>
       </c>
@@ -2582,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="11">
         <v>43104.833328009256</v>
       </c>
@@ -2602,7 +2635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="11">
         <v>43104.874994618054</v>
       </c>
@@ -2622,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="11">
         <v>43104.916661226853</v>
       </c>
@@ -2642,7 +2675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="11">
         <v>43104.958327835651</v>
       </c>
@@ -2662,7 +2695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="11">
         <v>43104.999994444443</v>
       </c>
@@ -2670,7 +2703,7 @@
         <v>3.9999999999999498</v>
       </c>
       <c r="C98" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D98" s="3">
         <f>0</f>
@@ -2685,7 +2718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="11">
         <v>43105.041661053241</v>
       </c>
@@ -2705,7 +2738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="11">
         <v>43105.08332766204</v>
       </c>
@@ -2725,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="11">
         <v>43105.124994270831</v>
       </c>
@@ -2745,7 +2778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="11">
         <v>43105.166660879629</v>
       </c>
@@ -2765,7 +2798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="11">
         <v>43105.208327488428</v>
       </c>
@@ -2785,7 +2818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="11">
         <v>43105.249994097219</v>
       </c>
@@ -2805,7 +2838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="11">
         <v>43105.291660706018</v>
       </c>
@@ -2825,7 +2858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="11">
         <v>43105.333327314816</v>
       </c>
@@ -2845,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="11">
         <v>43105.374993923608</v>
       </c>
@@ -2865,7 +2898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="11">
         <v>43105.416660532406</v>
       </c>
@@ -2885,7 +2918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="11">
         <v>43105.458327141205</v>
       </c>
@@ -2905,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="11">
         <v>43105.499993750003</v>
       </c>
@@ -2925,7 +2958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="11">
         <v>43105.541660358795</v>
       </c>
@@ -2945,7 +2978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="11">
         <v>43105.583326967593</v>
       </c>
@@ -2965,7 +2998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="11">
         <v>43105.624993576392</v>
       </c>
@@ -2985,7 +3018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="11">
         <v>43105.666660185183</v>
       </c>
@@ -3005,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="11">
         <v>43105.708326793982</v>
       </c>
@@ -3025,7 +3058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="11">
         <v>43105.74999340278</v>
       </c>
@@ -3045,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="11">
         <v>43105.791660011571</v>
       </c>
@@ -3065,7 +3098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="11">
         <v>43105.83332662037</v>
       </c>
@@ -3085,7 +3118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="11">
         <v>43105.874993229168</v>
       </c>
@@ -3105,7 +3138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="11">
         <v>43105.91665983796</v>
       </c>
@@ -3125,7 +3158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="11">
         <v>43105.958326446758</v>
       </c>
@@ -3145,7 +3178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="11">
         <v>43105.999993055557</v>
       </c>
@@ -3153,7 +3186,7 @@
         <v>4.9999999999999298</v>
       </c>
       <c r="C122" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D122" s="3">
         <f>0</f>
@@ -3168,7 +3201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="11">
         <v>43106.041659664355</v>
       </c>
@@ -3188,7 +3221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="11">
         <v>43106.083326273147</v>
       </c>
@@ -3208,7 +3241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="11">
         <v>43106.124992881945</v>
       </c>
@@ -3228,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="11">
         <v>43106.166659490744</v>
       </c>
@@ -3248,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="11">
         <v>43106.208326099535</v>
       </c>
@@ -3268,7 +3301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="11">
         <v>43106.249992708334</v>
       </c>
@@ -3288,7 +3321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="11">
         <v>43106.291659317132</v>
       </c>
@@ -3308,7 +3341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="11">
         <v>43106.333325925923</v>
       </c>
@@ -3328,7 +3361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="11">
         <v>43106.374992534722</v>
       </c>
@@ -3348,7 +3381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="11">
         <v>43106.416659143521</v>
       </c>
@@ -3368,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="11">
         <v>43106.458325752312</v>
       </c>
@@ -3388,7 +3421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="11">
         <v>43106.49999236111</v>
       </c>
@@ -3408,7 +3441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="11">
         <v>43106.541658969909</v>
       </c>
@@ -3428,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="11">
         <v>43106.5833255787</v>
       </c>
@@ -3448,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="11">
         <v>43106.624992187499</v>
       </c>
@@ -3468,7 +3501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="11">
         <v>43106.666658796297</v>
       </c>
@@ -3488,7 +3521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="11">
         <v>43106.708325405096</v>
       </c>
@@ -3508,7 +3541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="11">
         <v>43106.749992013887</v>
       </c>
@@ -3528,7 +3561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="11">
         <v>43106.791658622686</v>
       </c>
@@ -3548,7 +3581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="11">
         <v>43106.833325231484</v>
       </c>
@@ -3568,7 +3601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="11">
         <v>43106.874991840275</v>
       </c>
@@ -3588,7 +3621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="11">
         <v>43106.916658449074</v>
       </c>
@@ -3608,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="11">
         <v>43106.958325057873</v>
       </c>
@@ -3628,7 +3661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="11">
         <v>43106.999991666664</v>
       </c>
@@ -3636,7 +3669,7 @@
         <v>5.9999999999999103</v>
       </c>
       <c r="C146" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D146" s="3">
         <f>0</f>
@@ -3651,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="11">
         <v>43107.041658275462</v>
       </c>
@@ -3671,7 +3704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="11">
         <v>43107.083324884261</v>
       </c>
@@ -3691,7 +3724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="11">
         <v>43107.124991493052</v>
       </c>
@@ -3711,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="11">
         <v>43107.166658101851</v>
       </c>
@@ -3731,7 +3764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="11">
         <v>43107.208324710649</v>
       </c>
@@ -3751,7 +3784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="11">
         <v>43107.249991319448</v>
       </c>
@@ -3771,7 +3804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="11">
         <v>43107.291657928239</v>
       </c>
@@ -3791,7 +3824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="11">
         <v>43107.333324537038</v>
       </c>
@@ -3811,7 +3844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="11">
         <v>43107.374991145836</v>
       </c>
@@ -3831,7 +3864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="11">
         <v>43107.416657754628</v>
       </c>
@@ -3851,7 +3884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="11">
         <v>43107.458324363426</v>
       </c>
@@ -3871,7 +3904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="11">
         <v>43107.499990972225</v>
       </c>
@@ -3891,7 +3924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="11">
         <v>43107.541657581016</v>
       </c>
@@ -3911,7 +3944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="11">
         <v>43107.583324189814</v>
       </c>
@@ -3931,7 +3964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="11">
         <v>43107.624990798613</v>
       </c>
@@ -3951,7 +3984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="11">
         <v>43107.666657407404</v>
       </c>
@@ -3971,7 +4004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="11">
         <v>43107.708324016203</v>
       </c>
@@ -3991,7 +4024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="11">
         <v>43107.749990625001</v>
       </c>
@@ -4011,7 +4044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="11">
         <v>43107.7916572338</v>
       </c>
@@ -4031,7 +4064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="11">
         <v>43107.833323842591</v>
       </c>
@@ -4051,7 +4084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="11">
         <v>43107.87499045139</v>
       </c>
@@ -4071,7 +4104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="11">
         <v>43107.916657060188</v>
       </c>
@@ -4091,7 +4124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="11">
         <v>43107.95832366898</v>
       </c>
@@ -4123,72 +4156,73 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <f>K2*P2</f>
@@ -4247,9 +4281,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <f>D2+((F2*I2)/N2)*K2</f>
@@ -4284,9 +4318,9 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B4" s="8">
         <f>D3+((F3*I3)/N2)*K2</f>
@@ -4321,12 +4355,12 @@
         <v>3.7</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B5" s="8">
         <f>D4+((F4*I4)/N2)*K2</f>
@@ -4365,9 +4399,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B6" s="8">
         <f>D5+((F5*I5)/N2)*K2</f>
@@ -4402,7 +4436,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
@@ -4412,9 +4446,9 @@
       <c r="H7" s="7"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
         <f>(D6)+((F6*I6)/N2)*K2</f>
@@ -4449,9 +4483,9 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3">
         <f>D8+((F8*I8)/N2)*K2</f>
@@ -4486,31 +4520,31 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="6:6">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F20" s="5"/>
     </row>
-    <row r="22" spans="6:6">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F22">
         <f>(C2-E2)*N2</f>
         <v>14.224691358024691</v>
@@ -4525,78 +4559,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBC39DF-7100-4202-BE5F-35CFC9F04E32}">
   <dimension ref="A1:Q179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="7" width="13.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" customWidth="1"/>
+    <col min="15" max="15" width="18.5" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <f>K2*P2</f>
@@ -4655,9 +4689,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <f>D2+((F2*I2)/N2)*K2</f>
@@ -4692,9 +4726,9 @@
         <v>2.0320987654320986</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3">
         <f>D3+((F3*I3)/N2)*K2</f>
@@ -4729,12 +4763,12 @@
         <v>2.0320987654320986</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3">
         <f>D4+((F4*I4)/N2)*K2</f>
@@ -4773,9 +4807,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3">
         <f>D5+((F5*I5)/N2)*K2</f>
@@ -4810,7 +4844,7 @@
         <v>2.0320987654320986</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3"/>
@@ -4819,9 +4853,9 @@
       <c r="H7" s="6"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
         <f>D6+((F6*I6)/N2)*K2</f>
@@ -4857,9 +4891,9 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3">
         <f>D8</f>
@@ -4895,28 +4929,28 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="G14" t="s">
         <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="G15" s="3">
         <f>(L2/K2*N2)/F2</f>
@@ -4927,10 +4961,10 @@
         <v>0.54921588254921583</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
@@ -4942,10 +4976,10 @@
         <v>35</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="G18" s="3">
         <f>(L5/K2*N2)/F8</f>
@@ -4956,594 +4990,700 @@
         <v>0.64075186297408515</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="7"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="7"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="7"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="7"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="7"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="7"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="7"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="7"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="7"/>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="7"/>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="7"/>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="7"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="7"/>
       <c r="C84" s="3"/>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="7"/>
       <c r="C85" s="3"/>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="7"/>
       <c r="C86" s="3"/>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="7"/>
       <c r="C87" s="3"/>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="7"/>
       <c r="C88" s="3"/>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="7"/>
       <c r="C89" s="3"/>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="7"/>
       <c r="C90" s="3"/>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="7"/>
       <c r="C91" s="3"/>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="7"/>
       <c r="C92" s="3"/>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="7"/>
       <c r="C93" s="3"/>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="7"/>
       <c r="C94" s="3"/>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="7"/>
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="7"/>
       <c r="C96" s="3"/>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="7"/>
       <c r="C97" s="3"/>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="7"/>
       <c r="C98" s="3"/>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="C99" s="3"/>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="7"/>
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="7"/>
       <c r="C101" s="3"/>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="7"/>
       <c r="C102" s="3"/>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="7"/>
       <c r="C103" s="3"/>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="7"/>
       <c r="C104" s="3"/>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="7"/>
       <c r="C105" s="3"/>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="7"/>
       <c r="C107" s="3"/>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="7"/>
       <c r="C108" s="3"/>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="7"/>
       <c r="C109" s="3"/>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="7"/>
       <c r="C110" s="3"/>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="7"/>
       <c r="C111" s="3"/>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="7"/>
       <c r="C112" s="3"/>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="7"/>
       <c r="C113" s="3"/>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="7"/>
       <c r="C114" s="3"/>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="7"/>
       <c r="C115" s="3"/>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
       <c r="C116" s="3"/>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="7"/>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="7"/>
       <c r="C118" s="3"/>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
       <c r="C119" s="3"/>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="7"/>
       <c r="C120" s="3"/>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="7"/>
       <c r="C121" s="3"/>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="7"/>
       <c r="C122" s="3"/>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="7"/>
       <c r="C123" s="3"/>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="7"/>
       <c r="C124" s="3"/>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="7"/>
       <c r="C125" s="3"/>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="7"/>
       <c r="C126" s="3"/>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="7"/>
       <c r="C127" s="3"/>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="7"/>
       <c r="C128" s="3"/>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="7"/>
       <c r="C129" s="3"/>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="7"/>
       <c r="C130" s="3"/>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="7"/>
       <c r="C131" s="3"/>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="7"/>
       <c r="C132" s="3"/>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="7"/>
       <c r="C133" s="3"/>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="7"/>
       <c r="C134" s="3"/>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="7"/>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="7"/>
       <c r="C136" s="3"/>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="7"/>
       <c r="C137" s="3"/>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="7"/>
       <c r="C138" s="3"/>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="7"/>
       <c r="C139" s="3"/>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="7"/>
       <c r="C140" s="3"/>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="7"/>
       <c r="C141" s="3"/>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="7"/>
       <c r="C142" s="3"/>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="7"/>
       <c r="C143" s="3"/>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="7"/>
       <c r="C144" s="3"/>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="7"/>
       <c r="C145" s="3"/>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="7"/>
       <c r="C146" s="3"/>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="7"/>
       <c r="C147" s="3"/>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="7"/>
       <c r="C148" s="3"/>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="7"/>
       <c r="C149" s="3"/>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="7"/>
       <c r="C150" s="3"/>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="7"/>
       <c r="C151" s="3"/>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="7"/>
       <c r="C152" s="3"/>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="7"/>
       <c r="C153" s="3"/>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="7"/>
       <c r="C154" s="3"/>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="7"/>
       <c r="C155" s="3"/>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="7"/>
       <c r="C156" s="3"/>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="7"/>
       <c r="C157" s="3"/>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="7"/>
       <c r="C158" s="3"/>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="7"/>
       <c r="C159" s="3"/>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="7"/>
       <c r="C160" s="3"/>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="7"/>
       <c r="C161" s="3"/>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="7"/>
       <c r="C162" s="3"/>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="7"/>
       <c r="C163" s="3"/>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="7"/>
       <c r="C164" s="3"/>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="7"/>
       <c r="C165" s="3"/>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="7"/>
       <c r="C166" s="3"/>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="7"/>
       <c r="C167" s="3"/>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="7"/>
       <c r="C168" s="3"/>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="7"/>
       <c r="C169" s="3"/>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="7"/>
       <c r="C170" s="3"/>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="7"/>
       <c r="C171" s="3"/>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="7"/>
       <c r="C172" s="3"/>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="7"/>
       <c r="C173" s="3"/>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="7"/>
       <c r="C174" s="3"/>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="7"/>
       <c r="C175" s="3"/>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="7"/>
       <c r="C176" s="3"/>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="7"/>
       <c r="C177" s="3"/>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="7"/>
       <c r="C178" s="3"/>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="7"/>
       <c r="C179" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C41F1D-362D-9D40-9C19-D9939CCD42B4}">
+  <dimension ref="D7:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7">
+        <v>82.3</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <f>0.8*G7</f>
+        <v>65.84</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9">
+        <f>0.2*G7</f>
+        <v>16.46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11">
+        <f>E8-E9-E10</f>
+        <v>40.380000000000003</v>
+      </c>
+      <c r="G11">
+        <f>E11/G7</f>
+        <v>0.49064398541919813</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13">
+        <f>G7-E11</f>
+        <v>41.919999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14">
+        <v>3.7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15">
+        <f>E13/E14</f>
+        <v>11.329729729729728</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix EV_load power flow
</commit_message>
<xml_diff>
--- a/data/EV Calculation.xlsx
+++ b/data/EV Calculation.xlsx
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03086007-FF13-4F03-A8AB-B476DD27065A}">
   <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>